<commit_message>
DONALD-2 Addition of the categories vor parental employment status
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_DONALD_P2.xlsx
+++ b/rmonize/data_dictionary/DD_DONALD_P2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="143">
   <si>
     <t>index</t>
   </si>
@@ -428,6 +428,27 @@
   </si>
   <si>
     <t>noch in beruflicher Ausbildung (Auszubildener / Student)</t>
+  </si>
+  <si>
+    <t>employed-full time</t>
+  </si>
+  <si>
+    <t>employed-part time</t>
+  </si>
+  <si>
+    <t>housewife/-men</t>
+  </si>
+  <si>
+    <t>retired</t>
+  </si>
+  <si>
+    <t>unemployed</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -1584,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1915,24 +1936,101 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B30">
+      <c r="B37">
         <v>0</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C37" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B31">
+      <c r="B38">
         <v>1</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C38" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>